<commit_message>
show grid info on pointer, some refactor to dragging display
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC757B5-A708-4E52-A06F-04A86B4C3044}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD76729-0EA8-4404-B903-2251E17A0111}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -110,6 +110,48 @@
   </si>
   <si>
     <t>CLEAR</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>axisX</t>
+  </si>
+  <si>
+    <t>axisY</t>
+  </si>
+  <si>
+    <t>quadrant1</t>
+  </si>
+  <si>
+    <t>Quadrant 1</t>
+  </si>
+  <si>
+    <t>quadrant2</t>
+  </si>
+  <si>
+    <t>Quadrant 2</t>
+  </si>
+  <si>
+    <t>quadrant3</t>
+  </si>
+  <si>
+    <t>Quadrant 3</t>
+  </si>
+  <si>
+    <t>quadrant4</t>
+  </si>
+  <si>
+    <t>Quadrant 4</t>
+  </si>
+  <si>
+    <t>X - Axis</t>
+  </si>
+  <si>
+    <t>Y - Axis</t>
   </si>
 </sst>
 </file>
@@ -445,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +625,62 @@
         <v>29</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
revamp positioning on grid, initial hint display thing, some visuals
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD76729-0EA8-4404-B903-2251E17A0111}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBF5C13-9F85-487B-BA41-898B961C7DC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Key</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>Y - Axis</t>
+  </si>
+  <si>
+    <t>hintTooltip</t>
+  </si>
+  <si>
+    <t>Press this button to show hints.</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,6 +687,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
level 1 stuff, some progress logic, victory placeholder
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259A589-B8F4-47D2-925B-BB91EAD49BC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71194E-3DC7-4437-8F2D-C15B0E4A615B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16440" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Key</t>
   </si>
@@ -187,9 +187,6 @@
     <t>lesson1_0</t>
   </si>
   <si>
-    <t>The coordinate pair is made up of two lines: horizontal and vertical.</t>
-  </si>
-  <si>
     <t>lesson1_1</t>
   </si>
   <si>
@@ -232,22 +229,73 @@
     <t>...and the positive Y values go down.</t>
   </si>
   <si>
-    <t>When you pair the X and Y axis together, you get a coordinate.</t>
-  </si>
-  <si>
     <t>lesson1_9</t>
   </si>
   <si>
     <t>Next up, we will go over the quadrants.</t>
   </si>
   <si>
-    <t>The coordinate is a point where the X and Y axis intersect. Watch the coordinate change as Robert moves.</t>
-  </si>
-  <si>
     <t>dragItemTip</t>
   </si>
   <si>
     <t>Drag the item to the designated point.</t>
+  </si>
+  <si>
+    <t>playButtonTip</t>
+  </si>
+  <si>
+    <t>Press this button to play.</t>
+  </si>
+  <si>
+    <t>The coordinate plane is a two-dimensional surface made up of two lines: horizontal and vertical.</t>
+  </si>
+  <si>
+    <t>When you pair the X and Y values together, you get a point on the coordinate plane.</t>
+  </si>
+  <si>
+    <t>The point is where the two axis lines intersect. Watch the two values change as Robert moves.</t>
+  </si>
+  <si>
+    <t>lesson2_0</t>
+  </si>
+  <si>
+    <t>The quadrants are the four sections of the coordinate plane.</t>
+  </si>
+  <si>
+    <t>lesson2_1</t>
+  </si>
+  <si>
+    <t>lesson2_2</t>
+  </si>
+  <si>
+    <t>lesson2_3</t>
+  </si>
+  <si>
+    <t>lesson2_4</t>
+  </si>
+  <si>
+    <t>lesson2_5</t>
+  </si>
+  <si>
+    <t>lesson2_6</t>
+  </si>
+  <si>
+    <t>As you can see, the quadrants are divided by the X and Y axis from the origin.</t>
+  </si>
+  <si>
+    <t>Each one determines the sign values of the X and Y: positive or negative.</t>
+  </si>
+  <si>
+    <t>Now let's help Robert move from Quadrant 1 to Quadrant 2.</t>
+  </si>
+  <si>
+    <t>Nice! Next stop: Quadrant 3.</t>
+  </si>
+  <si>
+    <t>One last destination: Quadrant 4.</t>
+  </si>
+  <si>
+    <t>Excellent! Now we are ready to patch the system!</t>
   </si>
 </sst>
 </file>
@@ -583,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,90 +867,154 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
+        <v>73</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some color palettes, end scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E34C8ED-F600-4540-A416-B5A6A48C9A84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC916B52-9D90-4901-88E1-486DA5E5DD36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Key</t>
   </si>
@@ -355,9 +355,6 @@
     <t>intro_2</t>
   </si>
   <si>
-    <t>Excellent! With your guidance, he can finally move forward.</t>
-  </si>
-  <si>
     <t>lesson1_begin</t>
   </si>
   <si>
@@ -368,6 +365,27 @@
   </si>
   <si>
     <t>Escape From Quadrant</t>
+  </si>
+  <si>
+    <t>Excellent! With your guidance, Robert can finally move on.</t>
+  </si>
+  <si>
+    <t>end_0</t>
+  </si>
+  <si>
+    <t>After a long arduous journey, Robert is finally united with his family!</t>
+  </si>
+  <si>
+    <t>end_1</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -706,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +779,7 @@
         <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,10 +984,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1123,7 @@
         <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1134,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -1124,7 +1142,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -1132,7 +1150,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -1140,7 +1158,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -1148,7 +1166,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -1156,7 +1174,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -1172,7 +1190,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -1180,12 +1198,42 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added music and sound
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D96671-54E2-4BD6-B891-86CC859BFB8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBD2DA4-2E98-41E7-A710-2DBC0781A311}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Key</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>LEVEL COMPLETE</t>
+  </si>
+  <si>
+    <t>roger_roger</t>
+  </si>
+  <si>
+    <t>Roger! Roger!</t>
   </si>
 </sst>
 </file>
@@ -730,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,6 +1256,14 @@
         <v>123</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added grid line display, fixed typo in language
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7931C9E6-2AD3-4230-A548-985A2E214893}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1AF9E7-95D9-4901-9681-C4237C1DC9B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>Now, the vertical line: The Y-axis.</t>
   </si>
   <si>
-    <t>...and the positive Y values go down.</t>
-  </si>
-  <si>
     <t>lesson1_9</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>This is Robert. He has been running in circles for ages.</t>
+  </si>
+  <si>
+    <t>...and the negative Y values go down.</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,15 +777,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,26 +974,26 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
         <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1065,159 +1065,159 @@
         <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" t="s">
         <v>65</v>
-      </c>
-      <c r="B40" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
         <v>85</v>
-      </c>
-      <c r="B48" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
         <v>101</v>
-      </c>
-      <c r="B56" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
         <v>109</v>
-      </c>
-      <c r="B58" t="s">
-        <v>110</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
         <v>111</v>
-      </c>
-      <c r="B59" t="s">
-        <v>112</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -1236,18 +1236,18 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
         <v>113</v>
-      </c>
-      <c r="B60" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" t="s">
         <v>115</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated language with spanish stuff, also added tool to make it easier to re-integrate localization (should have done this months ago)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1A06DE-22C4-47F7-BC26-3B76C75879EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9AA7FD-996B-456C-94BC-9A2464B3DC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="189">
   <si>
     <t>Key</t>
   </si>
@@ -404,6 +405,189 @@
   </si>
   <si>
     <t>Which quadrant will Robert teleport in?</t>
+  </si>
+  <si>
+    <t>Bienvenido!</t>
+  </si>
+  <si>
+    <t>Escapar del cuadrante</t>
+  </si>
+  <si>
+    <t>CRÉDITOS</t>
+  </si>
+  <si>
+    <t>Escrito por: David Dionisio\nMúsica de: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>JUGAR</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>ENCENDIDO</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>CERCA</t>
+  </si>
+  <si>
+    <t>CLARO</t>
+  </si>
+  <si>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>El Eje X</t>
+  </si>
+  <si>
+    <t>El Eje Y</t>
+  </si>
+  <si>
+    <t>El Eje X (+)</t>
+  </si>
+  <si>
+    <t>El Eje X (-)</t>
+  </si>
+  <si>
+    <t>El Eje Y(+)</t>
+  </si>
+  <si>
+    <t>El Eje Y (-)</t>
+  </si>
+  <si>
+    <t>Cuadrante 1</t>
+  </si>
+  <si>
+    <t>Cuadrante 2</t>
+  </si>
+  <si>
+    <t>Cuadrante 3</t>
+  </si>
+  <si>
+    <t>Cuadrante 4</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para mostrar sugerencias.</t>
+  </si>
+  <si>
+    <t>Arrastre el elemento hasta el punto designado.</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para jugar.</t>
+  </si>
+  <si>
+    <t>Para ayudar a Robert aún más, primero debemos aprender sobre el plano de coordenadas.</t>
+  </si>
+  <si>
+    <t>El plano de coordenadas es una superficie bidimensional formada por dos líneas: horizontal y vertical.</t>
+  </si>
+  <si>
+    <t>Primero, la línea horizontal: el eje X.</t>
+  </si>
+  <si>
+    <t>A partir del origen, los valores X positivos van a la derecha.</t>
+  </si>
+  <si>
+    <t>... y los valores X negativos van a la izquierda.</t>
+  </si>
+  <si>
+    <t>Ahora, la línea vertical: el eje Y.</t>
+  </si>
+  <si>
+    <t>A partir del origen, los valores Y positivos suben.</t>
+  </si>
+  <si>
+    <t>... y los valores Y negativos bajan.</t>
+  </si>
+  <si>
+    <t>Cuando emparejas los valores X e Y juntos, obtendás una coordenada.</t>
+  </si>
+  <si>
+    <t>La coordenada es donde se cruzan las líneas de los ejes X e Y. Observa que los dos valores cambian a medida que Robert se mueve.</t>
+  </si>
+  <si>
+    <t>A continuación, repasaremos los cuadrantes.</t>
+  </si>
+  <si>
+    <t>Los cuadrantes son las cuatro secciones del plano de coordenadas.</t>
+  </si>
+  <si>
+    <t>Como puedes ver, los cuadrantes están divididos por los ejes X e Y desde el origen.</t>
+  </si>
+  <si>
+    <t>Cada uno determina los valores de signo del X e Y: positivos o negativos.</t>
+  </si>
+  <si>
+    <t>Ahora vamos a ayudar a Robert a pasar del cuadrante 1 al cuadrante 2.</t>
+  </si>
+  <si>
+    <t>¡Genial! El próximo paso: Cuadrante 3.</t>
+  </si>
+  <si>
+    <t>Un último destino: Cuadrante 4.</t>
+  </si>
+  <si>
+    <t>!Excelente! Ahora estás listo para guiar a Robert de vuelta a su familia.</t>
+  </si>
+  <si>
+    <t>Ahora vamos a repasar la reflexión.</t>
+  </si>
+  <si>
+    <t>Un punto se refleja al voltear los signos de sus valores: positivo a negativo y viceversa.</t>
+  </si>
+  <si>
+    <t>Aquí puedes ver el valor X reflejado en el eje Y.</t>
+  </si>
+  <si>
+    <t>... y el valor Y, que se refleja en el eje X.</t>
+  </si>
+  <si>
+    <t>Al reflejar los valores X e Y, puede ver que la línea que conecta ambos puntos recorre el origen.</t>
+  </si>
+  <si>
+    <t>Los dos puntos tienen la misma distancia del origen.</t>
+  </si>
+  <si>
+    <t>¡Ahora pongamos esto en práctica! Coloque los reflejos coincidentes en las fichas resaltadas.</t>
+  </si>
+  <si>
+    <t>Este es Robert. Ha estado corriendo en círculos durante años.</t>
+  </si>
+  <si>
+    <t>Por favor, rompe este ciclo para que pueda reunirse con su familia.</t>
+  </si>
+  <si>
+    <t>¡Excelente!  Con tu dirección, Robert finalmente puede seguir adelante.</t>
+  </si>
+  <si>
+    <t>Después de un largo y arduo viaje, Robert finalmente se une a su familia.</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>COMPLETO</t>
+  </si>
+  <si>
+    <t>NIVEL COMPLETO</t>
+  </si>
+  <si>
+    <t>CUADRANTE</t>
+  </si>
+  <si>
+    <t>¿En qué cuadrante se teletransportará Robert?</t>
   </si>
 </sst>
 </file>
@@ -744,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,4 +1466,548 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added "new game" and "continue"
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9AA7FD-996B-456C-94BC-9A2464B3DC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9B7088-75FB-4AB8-BC72-805E349729D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="195">
   <si>
     <t>Key</t>
   </si>
@@ -588,6 +588,24 @@
   </si>
   <si>
     <t>¿En qué cuadrante se teletransportará Robert?</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
   </si>
 </sst>
 </file>
@@ -926,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,455 +1028,471 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>189</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>190</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>104</v>
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" t="s">
-        <v>116</v>
+        <v>103</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1470,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,455 +1588,471 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>133</v>
+        <v>189</v>
+      </c>
+      <c r="B8" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>134</v>
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>155</v>
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>156</v>
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" t="s">
-        <v>157</v>
+        <v>103</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>176</v>
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" t="s">
-        <v>178</v>
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>183</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>184</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>188</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added coordinate question to alternate between quadrant question (it's really just the same thing), updated how-to description to match new hint system.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9B7088-75FB-4AB8-BC72-805E349729D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782BD228-2968-4927-84EA-C6E1D27FE43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="197">
   <si>
     <t>Key</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>coord_question</t>
+  </si>
+  <si>
+    <t>What coordinate will Robert teleport in?</t>
   </si>
 </sst>
 </file>
@@ -944,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,6 +1502,14 @@
         <v>127</v>
       </c>
     </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1504,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,6 +2070,11 @@
         <v>188</v>
       </c>
     </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added reflection question, fixed hint showing up incorrectly, added mock-up scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782BD228-2968-4927-84EA-C6E1D27FE43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D12046-6DB4-45C2-9EFF-9BEF091D835F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="199">
   <si>
     <t>Key</t>
   </si>
@@ -612,6 +612,12 @@
   </si>
   <si>
     <t>What coordinate will Robert teleport in?</t>
+  </si>
+  <si>
+    <t>reflect_question</t>
+  </si>
+  <si>
+    <t>What is the reflection of this coordinate?</t>
   </si>
 </sst>
 </file>
@@ -950,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,6 +1516,14 @@
         <v>196</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1518,7 +1532,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
@@ -2075,6 +2089,11 @@
         <v>195</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added new quadrant select modal for LO, various fixes here and there
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D12046-6DB4-45C2-9EFF-9BEF091D835F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D156B54E-7D1B-4A5C-85FE-A027B8E78CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1830" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9345" yWindow="4005" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="201">
   <si>
     <t>Key</t>
   </si>
@@ -611,13 +611,19 @@
     <t>coord_question</t>
   </si>
   <si>
-    <t>What coordinate will Robert teleport in?</t>
-  </si>
-  <si>
     <t>reflect_question</t>
   </si>
   <si>
     <t>What is the reflection of this coordinate?</t>
+  </si>
+  <si>
+    <t>deployment</t>
+  </si>
+  <si>
+    <t>DEPLOYMENT</t>
+  </si>
+  <si>
+    <t>Please verify the teleportation coordinate.</t>
   </si>
 </sst>
 </file>
@@ -956,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,16 +1518,24 @@
       <c r="A66" t="s">
         <v>195</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>196</v>
+      <c r="B66" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B67" s="3" t="s">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>198</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
@@ -2091,7 +2105,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modal coord numpad theoretically complete, initial work for modal deploy coord thing
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D156B54E-7D1B-4A5C-85FE-A027B8E78CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B11C7-3922-4980-8BBE-BEC4C5235DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9345" yWindow="4005" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="203">
   <si>
     <t>Key</t>
   </si>
@@ -624,6 +624,12 @@
   </si>
   <si>
     <t>Please verify the teleportation coordinate.</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
   </si>
 </sst>
 </file>
@@ -962,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,6 +1542,14 @@
       </c>
       <c r="B68" s="3" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>201</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial implements of ModalDeploymentCoord
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B11C7-3922-4980-8BBE-BEC4C5235DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86520D96-1759-473E-BE7F-DC12BA98FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9345" yWindow="4005" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="205">
   <si>
     <t>Key</t>
   </si>
@@ -630,6 +630,12 @@
   </si>
   <si>
     <t>VERIFY</t>
+  </si>
+  <si>
+    <t>out_of_bounds</t>
+  </si>
+  <si>
+    <t>Out of Bounds!</t>
   </si>
 </sst>
 </file>
@@ -968,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,6 +1556,14 @@
       </c>
       <c r="B69" s="3" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added dialog for deployment phase, some tweaks here and there, new submit build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86520D96-1759-473E-BE7F-DC12BA98FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCA3E48-E3BC-4583-88D6-6B25EADD0E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9345" yWindow="4005" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="4275" windowWidth="26865" windowHeight="13815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>Key</t>
   </si>
@@ -636,6 +636,42 @@
   </si>
   <si>
     <t>Out of Bounds!</t>
+  </si>
+  <si>
+    <t>deploy_quad_0</t>
+  </si>
+  <si>
+    <t>Before we begin, we must verify Robert's coordinates.</t>
+  </si>
+  <si>
+    <t>deploy_quad_1</t>
+  </si>
+  <si>
+    <t>deploy_coord_0</t>
+  </si>
+  <si>
+    <t>deploy_coord_1</t>
+  </si>
+  <si>
+    <t>deploy_coord_2</t>
+  </si>
+  <si>
+    <t>You can switch which coordinates to input by pressing the left or right arrow.</t>
+  </si>
+  <si>
+    <t>First, you must choose the correct quadrant.</t>
+  </si>
+  <si>
+    <t>deploy_coord_3</t>
+  </si>
+  <si>
+    <t>Once you are satisfied with the coordinate numbers, press the VERIFY button to proceed.</t>
+  </si>
+  <si>
+    <t>Excellent! Now we need to input the actual coordinate numbers.</t>
+  </si>
+  <si>
+    <t>Use the numpad to input the X and Y coordinates.</t>
   </si>
 </sst>
 </file>
@@ -974,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,6 +1602,54 @@
         <v>204</v>
       </c>
     </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>208</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>213</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1574,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6739EA66-881C-40E3-B210-882CB0383F57}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,6 +2220,51 @@
         <v>196</v>
       </c>
     </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>